<commit_message>
sql ana add get lowBidPrice first coming time, add ana into jpp60.xlsx
</commit_message>
<xml_diff>
--- a/jpp60.xlsx
+++ b/jpp60.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="480" windowWidth="19155" windowHeight="7260"/>
+    <workbookView xWindow="840" yWindow="480" windowWidth="19155" windowHeight="7260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="hq" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4309" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4311" uniqueCount="739">
   <si>
     <t>lprice</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2311,6 +2311,14 @@
     <t>jsprice</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>bS20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bS10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -2619,7 +2627,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2964,6 +2972,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - 强调文字颜色 1" xfId="4" builtinId="30"/>
@@ -3273,7 +3290,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E4160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2051" sqref="E2051"/>
     </sheetView>
@@ -3313,7 +3330,7 @@
         <v>85100</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:E65" si="0">C2-300</f>
+        <f t="shared" ref="D2:D65" si="0">C2-300</f>
         <v>84800</v>
       </c>
       <c r="E2" s="1">
@@ -75800,18 +75817,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="25" max="26" width="12" customWidth="1"/>
+    <col min="17" max="17" width="8.875" customWidth="1"/>
+    <col min="27" max="28" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -75825,106 +75843,113 @@
         <v>115</v>
       </c>
       <c r="E1" t="s">
+        <v>737</v>
+      </c>
+      <c r="F1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>95</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>96</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>97</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>98</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>99</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>100</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>101</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>102</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>738</v>
+      </c>
+      <c r="Q1" t="s">
         <v>103</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>104</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>105</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>106</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>107</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>108</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>109</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>110</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>111</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>112</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>123</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>124</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>113</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>114</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>116</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>117</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>128</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:34">
       <c r="A2">
         <v>201401</v>
       </c>
       <c r="B2">
         <v>900</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="122">
         <f>B2-D2</f>
         <v>0</v>
       </c>
       <c r="D2">
         <v>900</v>
       </c>
-      <c r="E2">
-        <v>600</v>
+      <c r="E2" s="122">
+        <f>D2-F2</f>
+        <v>300</v>
       </c>
       <c r="F2">
         <v>600</v>
@@ -75945,18 +75970,19 @@
         <v>600</v>
       </c>
       <c r="L2">
+        <v>600</v>
+      </c>
+      <c r="M2">
         <v>500</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>400</v>
-      </c>
-      <c r="N2">
-        <v>300</v>
       </c>
       <c r="O2">
         <v>300</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="122">
+        <f>F2-Q2</f>
         <v>300</v>
       </c>
       <c r="Q2">
@@ -75975,61 +76001,68 @@
         <v>300</v>
       </c>
       <c r="V2">
+        <v>300</v>
+      </c>
+      <c r="W2">
+        <v>300</v>
+      </c>
+      <c r="X2">
         <v>100</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>0</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>0</v>
       </c>
-      <c r="Y2" s="39">
+      <c r="AA2" s="39">
         <v>900</v>
       </c>
-      <c r="Z2" s="44">
-        <f>Y2+300</f>
+      <c r="AB2" s="44">
+        <f>AA2+300</f>
         <v>1200</v>
       </c>
-      <c r="AA2">
-        <f>O2/Y2</f>
+      <c r="AC2">
+        <f>Q2/AA2</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AB2">
-        <f>E2/Y2</f>
+      <c r="AD2">
+        <f>F2/AA2</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="AC2">
-        <f>D2/Y2</f>
+      <c r="AE2">
+        <f>D2/AA2</f>
         <v>1</v>
       </c>
-      <c r="AD2">
-        <f>1000/O2</f>
+      <c r="AF2">
+        <f>1000/Q2</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="AE2">
-        <f>2000/E2</f>
+      <c r="AG2">
+        <f>2000/F2</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="AF2">
+      <c r="AH2">
         <f>6000/D2</f>
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:34">
       <c r="A3">
         <v>201402</v>
       </c>
       <c r="B3">
         <v>600</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="122">
         <f t="shared" ref="C3:C30" si="0">B3-D3</f>
         <v>0</v>
       </c>
       <c r="D3">
         <v>600</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="122">
+        <f t="shared" ref="E3:E30" si="1">D3-F3</f>
         <v>300</v>
       </c>
       <c r="F3">
@@ -76062,20 +76095,21 @@
       <c r="O3">
         <v>300</v>
       </c>
-      <c r="P3">
-        <v>300</v>
+      <c r="P3" s="122">
+        <f t="shared" ref="P3:P30" si="2">F3-Q3</f>
+        <v>0</v>
       </c>
       <c r="Q3">
         <v>300</v>
       </c>
       <c r="R3">
+        <v>300</v>
+      </c>
+      <c r="S3">
+        <v>300</v>
+      </c>
+      <c r="T3">
         <v>100</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -76089,54 +76123,61 @@
       <c r="X3">
         <v>0</v>
       </c>
-      <c r="Y3" s="39">
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="39">
         <v>600</v>
       </c>
-      <c r="Z3" s="44">
-        <f t="shared" ref="Z3:Z26" si="1">Y3+300</f>
+      <c r="AB3" s="44">
+        <f t="shared" ref="AB3:AB30" si="3">AA3+300</f>
         <v>900</v>
       </c>
-      <c r="AA3">
-        <f t="shared" ref="AA3:AA26" si="2">O3/Y3</f>
+      <c r="AC3">
+        <f t="shared" ref="AC3:AC30" si="4">Q3/AA3</f>
         <v>0.5</v>
       </c>
-      <c r="AB3">
-        <f t="shared" ref="AB3:AB26" si="3">E3/Y3</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD30" si="5">F3/AA3</f>
         <v>0.5</v>
       </c>
-      <c r="AC3">
-        <f t="shared" ref="AC3:AC26" si="4">D3/Y3</f>
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE30" si="6">D3/AA3</f>
         <v>1</v>
       </c>
-      <c r="AD3">
-        <f t="shared" ref="AD3:AD26" si="5">1000/O3</f>
+      <c r="AF3">
+        <f t="shared" ref="AF3:AF30" si="7">1000/Q3</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="AE3">
-        <f t="shared" ref="AE3:AE26" si="6">2000/E3</f>
+      <c r="AG3">
+        <f t="shared" ref="AG3:AG30" si="8">2000/F3</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="AF3">
-        <f t="shared" ref="AF3:AF27" si="7">6000/D3</f>
+      <c r="AH3">
+        <f>6000/D3</f>
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:34">
       <c r="A4">
         <v>201403</v>
       </c>
       <c r="B4">
         <v>1200</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="122">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="D4">
         <v>900</v>
       </c>
-      <c r="E4">
-        <v>300</v>
+      <c r="E4" s="122">
+        <f t="shared" si="1"/>
+        <v>600</v>
       </c>
       <c r="F4">
         <v>300</v>
@@ -76160,25 +76201,26 @@
         <v>300</v>
       </c>
       <c r="M4">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="N4">
         <v>200</v>
       </c>
       <c r="O4">
-        <v>100</v>
-      </c>
-      <c r="P4">
-        <v>100</v>
+        <v>200</v>
+      </c>
+      <c r="P4" s="122">
+        <f t="shared" si="2"/>
+        <v>200</v>
       </c>
       <c r="Q4">
         <v>100</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -76195,54 +76237,61 @@
       <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y4" s="39">
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="39">
         <v>1200</v>
       </c>
-      <c r="Z4" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB4" s="44">
+        <f t="shared" si="3"/>
         <v>1500</v>
-      </c>
-      <c r="AA4">
-        <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="AB4">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
       </c>
       <c r="AC4">
         <f t="shared" si="4"/>
-        <v>0.75</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="AD4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>0.25</v>
       </c>
       <c r="AE4">
         <f t="shared" si="6"/>
-        <v>6.666666666666667</v>
+        <v>0.75</v>
       </c>
       <c r="AF4">
         <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" si="8"/>
         <v>6.666666666666667</v>
       </c>
-    </row>
-    <row r="5" spans="1:32">
+      <c r="AH4">
+        <f>6000/D4</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5">
         <v>201404</v>
       </c>
       <c r="B5">
         <v>1400</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="122">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="D5">
         <v>900</v>
       </c>
-      <c r="E5">
-        <v>500</v>
+      <c r="E5" s="122">
+        <f t="shared" si="1"/>
+        <v>400</v>
       </c>
       <c r="F5">
         <v>500</v>
@@ -76254,13 +76303,13 @@
         <v>500</v>
       </c>
       <c r="I5">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="J5">
         <v>300</v>
       </c>
       <c r="K5">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="L5">
         <v>200</v>
@@ -76274,8 +76323,9 @@
       <c r="O5">
         <v>200</v>
       </c>
-      <c r="P5">
-        <v>200</v>
+      <c r="P5" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
       </c>
       <c r="Q5">
         <v>200</v>
@@ -76290,10 +76340,10 @@
         <v>200</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -76301,63 +76351,70 @@
       <c r="X5">
         <v>0</v>
       </c>
-      <c r="Y5" s="39">
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="39">
         <v>1400</v>
       </c>
-      <c r="Z5" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB5" s="44">
+        <f t="shared" si="3"/>
         <v>1700</v>
-      </c>
-      <c r="AA5">
-        <f t="shared" si="2"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AB5">
-        <f t="shared" si="3"/>
-        <v>0.35714285714285715</v>
       </c>
       <c r="AC5">
         <f t="shared" si="4"/>
-        <v>0.6428571428571429</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="AD5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="AE5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="AF5">
         <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AH5">
+        <f>6000/D5</f>
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:34">
       <c r="A6">
         <v>201405</v>
       </c>
       <c r="B6">
         <v>1800</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="122">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="D6">
         <v>1200</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="122">
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
       <c r="F6">
+        <v>600</v>
+      </c>
+      <c r="G6">
         <v>500</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>400</v>
-      </c>
-      <c r="H6">
-        <v>300</v>
       </c>
       <c r="I6">
         <v>300</v>
@@ -76375,25 +76432,26 @@
         <v>300</v>
       </c>
       <c r="N6">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="O6">
         <v>200</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="122">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="Q6">
         <v>200</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
+        <v>200</v>
+      </c>
+      <c r="S6">
         <v>100</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>100</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -76407,53 +76465,60 @@
       <c r="X6">
         <v>0</v>
       </c>
-      <c r="Y6" s="39">
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="39">
         <v>1800</v>
       </c>
-      <c r="Z6" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB6" s="44">
+        <f t="shared" si="3"/>
         <v>2100</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="AB6">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
       </c>
       <c r="AC6">
         <f t="shared" si="4"/>
-        <v>0.66666666666666663</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="AD6">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AE6">
         <f t="shared" si="6"/>
-        <v>3.3333333333333335</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AF6">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:32">
+      <c r="AG6">
+        <f t="shared" si="8"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="AH6">
+        <f>6000/D6</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
       <c r="A7">
         <v>201406</v>
       </c>
       <c r="B7">
         <v>1200</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="122">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="D7">
         <v>600</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="122">
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="F7">
@@ -76484,19 +76549,20 @@
         <v>300</v>
       </c>
       <c r="O7">
+        <v>300</v>
+      </c>
+      <c r="P7" s="122">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="Q7">
         <v>200</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>200</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>100</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -76513,54 +76579,61 @@
       <c r="X7">
         <v>0</v>
       </c>
-      <c r="Y7" s="39">
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="39">
         <v>1200</v>
       </c>
-      <c r="Z7" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB7" s="44">
+        <f t="shared" si="3"/>
         <v>1500</v>
-      </c>
-      <c r="AA7">
-        <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="AB7">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
       </c>
       <c r="AC7">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="AD7">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="AE7">
         <f t="shared" si="6"/>
-        <v>6.666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AF7">
         <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="8"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="AH7">
+        <f>6000/D7</f>
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:34">
       <c r="A8">
         <v>201407</v>
       </c>
       <c r="B8">
         <v>2000</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="122">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="D8">
         <v>1300</v>
       </c>
-      <c r="E8">
-        <v>400</v>
+      <c r="E8" s="122">
+        <f t="shared" si="1"/>
+        <v>900</v>
       </c>
       <c r="F8">
         <v>400</v>
@@ -76572,7 +76645,7 @@
         <v>400</v>
       </c>
       <c r="I8">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="J8">
         <v>300</v>
@@ -76587,12 +76660,13 @@
         <v>300</v>
       </c>
       <c r="N8">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="O8">
         <v>200</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="122">
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="Q8">
@@ -76605,10 +76679,10 @@
         <v>200</v>
       </c>
       <c r="T8">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="U8">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="V8">
         <v>100</v>
@@ -76619,54 +76693,61 @@
       <c r="X8">
         <v>100</v>
       </c>
-      <c r="Y8" s="39">
+      <c r="Y8">
+        <v>100</v>
+      </c>
+      <c r="Z8">
+        <v>100</v>
+      </c>
+      <c r="AA8" s="39">
         <v>2000</v>
       </c>
-      <c r="Z8" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB8" s="44">
+        <f t="shared" si="3"/>
         <v>2300</v>
-      </c>
-      <c r="AA8">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="AB8">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
       </c>
       <c r="AC8">
         <f t="shared" si="4"/>
-        <v>0.65</v>
+        <v>0.1</v>
       </c>
       <c r="AD8">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="AE8">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0.65</v>
       </c>
       <c r="AF8">
         <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AH8">
+        <f>6000/D8</f>
         <v>4.615384615384615</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:34">
       <c r="A9">
         <v>201408</v>
       </c>
       <c r="B9">
         <v>1000</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="122">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="D9">
         <v>700</v>
       </c>
-      <c r="E9">
-        <v>400</v>
+      <c r="E9" s="122">
+        <f t="shared" si="1"/>
+        <v>300</v>
       </c>
       <c r="F9">
         <v>400</v>
@@ -76675,19 +76756,19 @@
         <v>400</v>
       </c>
       <c r="H9">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="I9">
         <v>300</v>
       </c>
       <c r="J9">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="K9">
         <v>200</v>
       </c>
       <c r="L9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M9">
         <v>100</v>
@@ -76698,8 +76779,9 @@
       <c r="O9">
         <v>100</v>
       </c>
-      <c r="P9">
-        <v>100</v>
+      <c r="P9" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
       </c>
       <c r="Q9">
         <v>100</v>
@@ -76720,62 +76802,69 @@
         <v>100</v>
       </c>
       <c r="W9">
+        <v>100</v>
+      </c>
+      <c r="X9">
+        <v>100</v>
+      </c>
+      <c r="Y9">
         <v>0</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>0</v>
       </c>
-      <c r="Y9" s="39">
+      <c r="AA9" s="39">
         <v>1000</v>
       </c>
-      <c r="Z9" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB9" s="44">
+        <f t="shared" si="3"/>
         <v>1300</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="AB9">
-        <f t="shared" si="3"/>
-        <v>0.4</v>
       </c>
       <c r="AC9">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="AD9">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>0.4</v>
       </c>
       <c r="AE9">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0.7</v>
       </c>
       <c r="AF9">
         <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AH9">
+        <f>6000/D9</f>
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:34">
       <c r="A10">
         <v>201409</v>
       </c>
       <c r="B10">
         <v>1200</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="122">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="D10">
         <v>900</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="122">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="F10">
         <v>500</v>
-      </c>
-      <c r="F10">
-        <v>400</v>
       </c>
       <c r="G10">
         <v>400</v>
@@ -76784,7 +76873,7 @@
         <v>400</v>
       </c>
       <c r="I10">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="J10">
         <v>300</v>
@@ -76804,8 +76893,9 @@
       <c r="O10">
         <v>300</v>
       </c>
-      <c r="P10">
-        <v>300</v>
+      <c r="P10" s="122">
+        <f t="shared" si="2"/>
+        <v>200</v>
       </c>
       <c r="Q10">
         <v>300</v>
@@ -76814,71 +76904,78 @@
         <v>300</v>
       </c>
       <c r="S10">
+        <v>300</v>
+      </c>
+      <c r="T10">
+        <v>300</v>
+      </c>
+      <c r="U10">
         <v>200</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>100</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <v>100</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
       </c>
       <c r="X10">
         <v>0</v>
       </c>
-      <c r="Y10" s="39">
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="39">
         <v>1200</v>
       </c>
-      <c r="Z10" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB10" s="44">
+        <f t="shared" si="3"/>
         <v>1500</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="AB10">
-        <f t="shared" si="3"/>
-        <v>0.41666666666666669</v>
       </c>
       <c r="AC10">
         <f t="shared" si="4"/>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="AD10">
         <f t="shared" si="5"/>
-        <v>3.3333333333333335</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="AE10">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>0.75</v>
       </c>
       <c r="AF10">
         <f t="shared" si="7"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AH10">
+        <f>6000/D10</f>
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:34">
       <c r="A11">
         <v>201410</v>
       </c>
       <c r="B11">
         <v>1400</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="122">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="D11">
         <v>1100</v>
       </c>
-      <c r="E11">
-        <v>500</v>
+      <c r="E11" s="122">
+        <f t="shared" si="1"/>
+        <v>600</v>
       </c>
       <c r="F11">
         <v>500</v>
@@ -76893,7 +76990,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="K11">
         <v>400</v>
@@ -76902,16 +76999,17 @@
         <v>400</v>
       </c>
       <c r="M11">
+        <v>400</v>
+      </c>
+      <c r="N11">
         <v>300</v>
-      </c>
-      <c r="N11">
-        <v>200</v>
       </c>
       <c r="O11">
         <v>200</v>
       </c>
-      <c r="P11">
-        <v>200</v>
+      <c r="P11" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
       </c>
       <c r="Q11">
         <v>200</v>
@@ -76926,10 +77024,10 @@
         <v>200</v>
       </c>
       <c r="U11">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="V11">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="W11">
         <v>100</v>
@@ -76937,54 +77035,61 @@
       <c r="X11">
         <v>100</v>
       </c>
-      <c r="Y11" s="39">
+      <c r="Y11">
+        <v>100</v>
+      </c>
+      <c r="Z11">
+        <v>100</v>
+      </c>
+      <c r="AA11" s="39">
         <v>1400</v>
       </c>
-      <c r="Z11" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB11" s="44">
+        <f t="shared" si="3"/>
         <v>1700</v>
-      </c>
-      <c r="AA11">
-        <f t="shared" si="2"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AB11">
-        <f t="shared" si="3"/>
-        <v>0.35714285714285715</v>
       </c>
       <c r="AC11">
         <f t="shared" si="4"/>
-        <v>0.7857142857142857</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="AD11">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="AE11">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="AF11">
         <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AH11">
+        <f>6000/D11</f>
         <v>5.4545454545454541</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:34">
       <c r="A12">
         <v>201411</v>
       </c>
       <c r="B12">
         <v>900</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="122">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="D12">
         <v>600</v>
       </c>
-      <c r="E12">
-        <v>600</v>
+      <c r="E12" s="122">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>600</v>
@@ -77002,10 +77107,10 @@
         <v>600</v>
       </c>
       <c r="K12">
+        <v>600</v>
+      </c>
+      <c r="L12">
         <v>400</v>
-      </c>
-      <c r="L12">
-        <v>300</v>
       </c>
       <c r="M12">
         <v>300</v>
@@ -77016,26 +77121,27 @@
       <c r="O12">
         <v>300</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="122">
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="Q12">
+        <v>300</v>
+      </c>
+      <c r="R12">
+        <v>300</v>
+      </c>
+      <c r="S12">
         <v>200</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>200</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>100</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>100</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -77043,54 +77149,61 @@
       <c r="X12">
         <v>0</v>
       </c>
-      <c r="Y12" s="39">
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="39">
         <v>900</v>
       </c>
-      <c r="Z12" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB12" s="44">
+        <f t="shared" si="3"/>
         <v>1200</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="AB12">
-        <f t="shared" si="3"/>
-        <v>0.66666666666666663</v>
       </c>
       <c r="AC12">
         <f t="shared" si="4"/>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AD12">
         <f t="shared" si="5"/>
-        <v>3.3333333333333335</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AE12">
         <f t="shared" si="6"/>
-        <v>3.3333333333333335</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AF12">
         <f t="shared" si="7"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="8"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="AH12">
+        <f>6000/D12</f>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:34">
       <c r="A13">
         <v>201412</v>
       </c>
       <c r="B13">
         <v>1000</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="122">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="D13">
         <v>700</v>
       </c>
-      <c r="E13">
-        <v>700</v>
+      <c r="E13" s="122">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>700</v>
@@ -77099,16 +77212,16 @@
         <v>700</v>
       </c>
       <c r="H13">
+        <v>700</v>
+      </c>
+      <c r="I13">
         <v>600</v>
-      </c>
-      <c r="I13">
-        <v>500</v>
       </c>
       <c r="J13">
         <v>500</v>
       </c>
       <c r="K13">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="L13">
         <v>400</v>
@@ -77122,20 +77235,21 @@
       <c r="O13">
         <v>400</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="Q13">
         <v>400</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
+        <v>400</v>
+      </c>
+      <c r="S13">
         <v>300</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>200</v>
-      </c>
-      <c r="S13">
-        <v>100</v>
-      </c>
-      <c r="T13">
-        <v>100</v>
       </c>
       <c r="U13">
         <v>100</v>
@@ -77147,56 +77261,63 @@
         <v>100</v>
       </c>
       <c r="X13">
+        <v>100</v>
+      </c>
+      <c r="Y13">
+        <v>100</v>
+      </c>
+      <c r="Z13">
         <v>0</v>
       </c>
-      <c r="Y13" s="39">
+      <c r="AA13" s="39">
         <v>1000</v>
       </c>
-      <c r="Z13" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB13" s="44">
+        <f t="shared" si="3"/>
         <v>1300</v>
-      </c>
-      <c r="AA13">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-      <c r="AB13">
-        <f t="shared" si="3"/>
-        <v>0.7</v>
       </c>
       <c r="AC13">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="AD13">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>0.7</v>
       </c>
       <c r="AE13">
         <f t="shared" si="6"/>
-        <v>2.8571428571428572</v>
+        <v>0.7</v>
       </c>
       <c r="AF13">
         <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="8"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="AH13">
+        <f>6000/D13</f>
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:34">
       <c r="A14">
         <v>201502</v>
       </c>
       <c r="B14">
         <v>2800</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="122">
         <f t="shared" si="0"/>
         <v>2300</v>
       </c>
       <c r="D14">
         <v>500</v>
       </c>
-      <c r="E14">
-        <v>300</v>
+      <c r="E14" s="122">
+        <f t="shared" si="1"/>
+        <v>200</v>
       </c>
       <c r="F14">
         <v>300</v>
@@ -77214,7 +77335,7 @@
         <v>300</v>
       </c>
       <c r="K14">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="L14">
         <v>200</v>
@@ -77228,8 +77349,9 @@
       <c r="O14">
         <v>200</v>
       </c>
-      <c r="P14">
-        <v>200</v>
+      <c r="P14" s="122">
+        <f t="shared" si="2"/>
+        <v>100</v>
       </c>
       <c r="Q14">
         <v>200</v>
@@ -77238,10 +77360,10 @@
         <v>200</v>
       </c>
       <c r="S14">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="T14">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="U14">
         <v>100</v>
@@ -77250,59 +77372,66 @@
         <v>100</v>
       </c>
       <c r="W14">
+        <v>100</v>
+      </c>
+      <c r="X14">
+        <v>100</v>
+      </c>
+      <c r="Y14">
         <v>0</v>
       </c>
-      <c r="X14">
+      <c r="Z14">
         <v>0</v>
       </c>
-      <c r="Y14" s="39">
+      <c r="AA14" s="39">
         <v>2800</v>
       </c>
-      <c r="Z14" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB14" s="44">
+        <f t="shared" si="3"/>
         <v>3100</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="2"/>
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="AB14">
-        <f t="shared" si="3"/>
-        <v>0.10714285714285714</v>
       </c>
       <c r="AC14">
         <f t="shared" si="4"/>
-        <v>0.17857142857142858</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="AD14">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0.10714285714285714</v>
       </c>
       <c r="AE14">
         <f t="shared" si="6"/>
-        <v>6.666666666666667</v>
+        <v>0.17857142857142858</v>
       </c>
       <c r="AF14">
         <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AG14">
+        <f t="shared" si="8"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="AH14">
+        <f>6000/D14</f>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:34">
       <c r="A15">
         <v>201504</v>
       </c>
       <c r="B15">
         <v>5400</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="122">
         <f t="shared" si="0"/>
         <v>4700</v>
       </c>
       <c r="D15">
         <v>700</v>
       </c>
-      <c r="E15">
-        <v>300</v>
+      <c r="E15" s="122">
+        <f t="shared" si="1"/>
+        <v>400</v>
       </c>
       <c r="F15">
         <v>300</v>
@@ -77329,28 +77458,29 @@
         <v>300</v>
       </c>
       <c r="N15">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="O15">
         <v>200</v>
       </c>
-      <c r="P15">
-        <v>200</v>
+      <c r="P15" s="122">
+        <f t="shared" si="2"/>
+        <v>100</v>
       </c>
       <c r="Q15">
         <v>200</v>
       </c>
       <c r="R15">
+        <v>200</v>
+      </c>
+      <c r="S15">
+        <v>200</v>
+      </c>
+      <c r="T15">
         <v>100</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>100</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -77361,54 +77491,61 @@
       <c r="X15">
         <v>0</v>
       </c>
-      <c r="Y15" s="39">
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="39">
         <v>5400</v>
       </c>
-      <c r="Z15" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB15" s="44">
+        <f t="shared" si="3"/>
         <v>5700</v>
-      </c>
-      <c r="AA15">
-        <f t="shared" si="2"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="AB15">
-        <f t="shared" si="3"/>
-        <v>5.5555555555555552E-2</v>
       </c>
       <c r="AC15">
         <f t="shared" si="4"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
       <c r="AD15">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="AE15">
         <f t="shared" si="6"/>
-        <v>6.666666666666667</v>
+        <v>0.12962962962962962</v>
       </c>
       <c r="AF15">
         <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="8"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="AH15">
+        <f>6000/D15</f>
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:34">
       <c r="A16">
         <v>201505</v>
       </c>
       <c r="B16">
         <v>3800</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="122">
         <f t="shared" si="0"/>
         <v>3100</v>
       </c>
       <c r="D16">
         <v>700</v>
       </c>
-      <c r="E16">
-        <v>300</v>
+      <c r="E16" s="122">
+        <f t="shared" si="1"/>
+        <v>400</v>
       </c>
       <c r="F16">
         <v>300</v>
@@ -77417,7 +77554,7 @@
         <v>300</v>
       </c>
       <c r="H16">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="I16">
         <v>200</v>
@@ -77440,11 +77577,12 @@
       <c r="O16">
         <v>200</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="122">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="Q16">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="R16">
         <v>100</v>
@@ -77465,62 +77603,69 @@
         <v>100</v>
       </c>
       <c r="X16">
+        <v>100</v>
+      </c>
+      <c r="Y16">
+        <v>100</v>
+      </c>
+      <c r="Z16">
         <v>0</v>
       </c>
-      <c r="Y16" s="39">
+      <c r="AA16" s="39">
         <v>3800</v>
       </c>
-      <c r="Z16" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB16" s="44">
+        <f t="shared" si="3"/>
         <v>4100</v>
-      </c>
-      <c r="AA16">
-        <f t="shared" si="2"/>
-        <v>5.2631578947368418E-2</v>
-      </c>
-      <c r="AB16">
-        <f t="shared" si="3"/>
-        <v>7.8947368421052627E-2</v>
       </c>
       <c r="AC16">
         <f t="shared" si="4"/>
-        <v>0.18421052631578946</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="AD16">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="AE16">
         <f t="shared" si="6"/>
-        <v>6.666666666666667</v>
+        <v>0.18421052631578946</v>
       </c>
       <c r="AF16">
         <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" si="8"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="AH16">
+        <f>6000/D16</f>
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="17" spans="1:32" s="46" customFormat="1">
+    <row r="17" spans="1:34" s="46" customFormat="1">
       <c r="A17" s="46">
         <v>201506</v>
       </c>
       <c r="B17" s="46">
         <v>4800</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="122">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="D17" s="46">
         <v>2300</v>
       </c>
-      <c r="E17" s="46">
-        <v>900</v>
+      <c r="E17" s="122">
+        <f t="shared" si="1"/>
+        <v>1400</v>
       </c>
       <c r="F17" s="46">
         <v>900</v>
       </c>
       <c r="G17" s="46">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="H17" s="46">
         <v>800</v>
@@ -77529,16 +77674,16 @@
         <v>800</v>
       </c>
       <c r="J17" s="46">
+        <v>800</v>
+      </c>
+      <c r="K17" s="46">
         <v>700</v>
-      </c>
-      <c r="K17" s="46">
-        <v>600</v>
       </c>
       <c r="L17" s="46">
         <v>600</v>
       </c>
       <c r="M17" s="46">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="N17" s="46">
         <v>500</v>
@@ -77546,93 +77691,101 @@
       <c r="O17" s="46">
         <v>500</v>
       </c>
-      <c r="P17" s="46">
+      <c r="P17" s="122">
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="Q17" s="46">
+        <v>500</v>
+      </c>
+      <c r="R17" s="46">
         <v>400</v>
       </c>
-      <c r="R17" s="46">
-        <v>300</v>
-      </c>
       <c r="S17" s="46">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="T17" s="46">
         <v>300</v>
       </c>
       <c r="U17" s="46">
+        <v>300</v>
+      </c>
+      <c r="V17" s="46">
+        <v>300</v>
+      </c>
+      <c r="W17" s="46">
         <v>200</v>
-      </c>
-      <c r="V17" s="46">
-        <v>100</v>
-      </c>
-      <c r="W17" s="46">
-        <v>100</v>
       </c>
       <c r="X17" s="46">
         <v>100</v>
       </c>
-      <c r="Y17" s="47">
+      <c r="Y17" s="46">
+        <v>100</v>
+      </c>
+      <c r="Z17" s="46">
+        <v>100</v>
+      </c>
+      <c r="AA17" s="47">
         <v>4800</v>
       </c>
-      <c r="Z17" s="48">
-        <f t="shared" si="1"/>
+      <c r="AB17" s="48">
+        <f t="shared" si="3"/>
         <v>5100</v>
-      </c>
-      <c r="AA17" s="46">
-        <f t="shared" si="2"/>
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="AB17" s="46">
-        <f t="shared" si="3"/>
-        <v>0.1875</v>
       </c>
       <c r="AC17" s="46">
         <f t="shared" si="4"/>
-        <v>0.47916666666666669</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="AD17" s="46">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0.1875</v>
       </c>
       <c r="AE17" s="46">
         <f t="shared" si="6"/>
-        <v>2.2222222222222223</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="AF17" s="46">
         <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="AG17" s="46">
+        <f t="shared" si="8"/>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="AH17" s="46">
+        <f>6000/D17</f>
         <v>2.6086956521739131</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:34">
       <c r="A18">
         <v>201507</v>
       </c>
       <c r="B18">
         <v>3200</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="122">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
       <c r="D18">
         <v>1700</v>
       </c>
-      <c r="E18">
-        <v>800</v>
+      <c r="E18" s="122">
+        <f t="shared" si="1"/>
+        <v>900</v>
       </c>
       <c r="F18">
         <v>800</v>
       </c>
       <c r="G18">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="H18">
         <v>700</v>
       </c>
       <c r="I18">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="J18">
         <v>600</v>
@@ -77641,7 +77794,7 @@
         <v>600</v>
       </c>
       <c r="L18">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="M18">
         <v>500</v>
@@ -77650,25 +77803,26 @@
         <v>500</v>
       </c>
       <c r="O18">
+        <v>500</v>
+      </c>
+      <c r="P18" s="122">
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
-      <c r="P18">
-        <v>300</v>
-      </c>
       <c r="Q18">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="R18">
         <v>300</v>
       </c>
       <c r="S18">
+        <v>300</v>
+      </c>
+      <c r="T18">
+        <v>300</v>
+      </c>
+      <c r="U18">
         <v>200</v>
-      </c>
-      <c r="T18">
-        <v>100</v>
-      </c>
-      <c r="U18">
-        <v>100</v>
       </c>
       <c r="V18">
         <v>100</v>
@@ -77677,56 +77831,63 @@
         <v>100</v>
       </c>
       <c r="X18">
+        <v>100</v>
+      </c>
+      <c r="Y18">
+        <v>100</v>
+      </c>
+      <c r="Z18">
         <v>0</v>
       </c>
-      <c r="Y18" s="39">
+      <c r="AA18" s="39">
         <v>3200</v>
       </c>
-      <c r="Z18" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB18" s="44">
+        <f t="shared" si="3"/>
         <v>3500</v>
-      </c>
-      <c r="AA18">
-        <f t="shared" si="2"/>
-        <v>0.125</v>
-      </c>
-      <c r="AB18">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
       </c>
       <c r="AC18">
         <f t="shared" si="4"/>
-        <v>0.53125</v>
+        <v>0.125</v>
       </c>
       <c r="AD18">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>0.25</v>
       </c>
       <c r="AE18">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>0.53125</v>
       </c>
       <c r="AF18">
         <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="AH18">
+        <f>6000/D18</f>
         <v>3.5294117647058822</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:34">
       <c r="A19">
         <v>201508</v>
       </c>
       <c r="B19">
         <v>2700</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="122">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="D19">
         <v>1500</v>
       </c>
-      <c r="E19">
-        <v>800</v>
+      <c r="E19" s="122">
+        <f t="shared" si="1"/>
+        <v>700</v>
       </c>
       <c r="F19">
         <v>800</v>
@@ -77735,7 +77896,7 @@
         <v>800</v>
       </c>
       <c r="H19">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I19">
         <v>700</v>
@@ -77744,7 +77905,7 @@
         <v>700</v>
       </c>
       <c r="K19">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="L19">
         <v>600</v>
@@ -77756,83 +77917,91 @@
         <v>600</v>
       </c>
       <c r="O19">
+        <v>600</v>
+      </c>
+      <c r="P19" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="Q19">
         <v>500</v>
       </c>
-      <c r="P19">
+      <c r="R19">
         <v>500</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>400</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <v>400</v>
       </c>
-      <c r="S19">
+      <c r="U19">
         <v>300</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>200</v>
-      </c>
-      <c r="U19">
-        <v>100</v>
-      </c>
-      <c r="V19">
-        <v>100</v>
       </c>
       <c r="W19">
         <v>100</v>
       </c>
       <c r="X19">
+        <v>100</v>
+      </c>
+      <c r="Y19">
+        <v>100</v>
+      </c>
+      <c r="Z19">
         <v>0</v>
       </c>
-      <c r="Y19" s="39">
+      <c r="AA19" s="39">
         <v>2700</v>
       </c>
-      <c r="Z19" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB19" s="44">
+        <f t="shared" si="3"/>
         <v>3000</v>
-      </c>
-      <c r="AA19">
-        <f t="shared" si="2"/>
-        <v>0.18518518518518517</v>
-      </c>
-      <c r="AB19">
-        <f t="shared" si="3"/>
-        <v>0.29629629629629628</v>
       </c>
       <c r="AC19">
         <f t="shared" si="4"/>
-        <v>0.55555555555555558</v>
+        <v>0.18518518518518517</v>
       </c>
       <c r="AD19">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0.29629629629629628</v>
       </c>
       <c r="AE19">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="AF19">
         <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="AG19">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="AH19">
+        <f>6000/D19</f>
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:34">
       <c r="A20">
         <v>201509</v>
       </c>
       <c r="B20">
         <v>2200</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="122">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="D20">
         <v>1300</v>
       </c>
-      <c r="E20">
-        <v>700</v>
+      <c r="E20" s="122">
+        <f t="shared" si="1"/>
+        <v>600</v>
       </c>
       <c r="F20">
         <v>700</v>
@@ -77844,7 +78013,7 @@
         <v>700</v>
       </c>
       <c r="I20">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="J20">
         <v>600</v>
@@ -77856,89 +78025,97 @@
         <v>600</v>
       </c>
       <c r="M20">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="N20">
         <v>500</v>
       </c>
       <c r="O20">
-        <v>400</v>
-      </c>
-      <c r="P20">
-        <v>400</v>
+        <v>500</v>
+      </c>
+      <c r="P20" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
       </c>
       <c r="Q20">
         <v>400</v>
       </c>
       <c r="R20">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="S20">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="T20">
         <v>300</v>
       </c>
       <c r="U20">
+        <v>300</v>
+      </c>
+      <c r="V20">
+        <v>300</v>
+      </c>
+      <c r="W20">
         <v>200</v>
-      </c>
-      <c r="V20">
-        <v>100</v>
-      </c>
-      <c r="W20">
-        <v>100</v>
       </c>
       <c r="X20">
         <v>100</v>
       </c>
-      <c r="Y20" s="39">
+      <c r="Y20">
+        <v>100</v>
+      </c>
+      <c r="Z20">
+        <v>100</v>
+      </c>
+      <c r="AA20" s="39">
         <v>2200</v>
       </c>
-      <c r="Z20" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB20" s="44">
+        <f t="shared" si="3"/>
         <v>2500</v>
-      </c>
-      <c r="AA20">
-        <f t="shared" si="2"/>
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="AB20">
-        <f t="shared" si="3"/>
-        <v>0.31818181818181818</v>
       </c>
       <c r="AC20">
         <f t="shared" si="4"/>
-        <v>0.59090909090909094</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="AD20">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>0.31818181818181818</v>
       </c>
       <c r="AE20">
         <f t="shared" si="6"/>
-        <v>2.8571428571428572</v>
+        <v>0.59090909090909094</v>
       </c>
       <c r="AF20">
         <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" si="8"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="AH20">
+        <f>6000/D20</f>
         <v>4.615384615384615</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:34">
       <c r="A21">
         <v>201510</v>
       </c>
       <c r="B21">
         <v>2700</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="122">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="D21">
         <v>1500</v>
       </c>
-      <c r="E21">
-        <v>800</v>
+      <c r="E21" s="122">
+        <f t="shared" si="1"/>
+        <v>700</v>
       </c>
       <c r="F21">
         <v>800</v>
@@ -77947,7 +78124,7 @@
         <v>800</v>
       </c>
       <c r="H21">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I21">
         <v>700</v>
@@ -77956,95 +78133,103 @@
         <v>700</v>
       </c>
       <c r="K21">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="L21">
         <v>600</v>
       </c>
       <c r="M21">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="N21">
         <v>500</v>
       </c>
       <c r="O21">
+        <v>500</v>
+      </c>
+      <c r="P21" s="122">
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>400</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
+        <v>400</v>
+      </c>
+      <c r="S21">
         <v>300</v>
       </c>
-      <c r="R21">
+      <c r="T21">
         <v>300</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <v>200</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>100</v>
       </c>
-      <c r="U21">
+      <c r="W21">
         <v>100</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
       </c>
       <c r="X21">
         <v>0</v>
       </c>
-      <c r="Y21" s="39">
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="39">
         <v>2700</v>
       </c>
-      <c r="Z21" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB21" s="44">
+        <f t="shared" si="3"/>
         <v>3000</v>
-      </c>
-      <c r="AA21">
-        <f t="shared" si="2"/>
-        <v>0.14814814814814814</v>
-      </c>
-      <c r="AB21">
-        <f t="shared" si="3"/>
-        <v>0.29629629629629628</v>
       </c>
       <c r="AC21">
         <f t="shared" si="4"/>
-        <v>0.55555555555555558</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="AD21">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>0.29629629629629628</v>
       </c>
       <c r="AE21">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="AF21">
         <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="AG21">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="AH21">
+        <f>6000/D21</f>
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:32" s="41" customFormat="1">
+    <row r="22" spans="1:34" s="41" customFormat="1">
       <c r="A22" s="41">
         <v>201511</v>
       </c>
       <c r="B22" s="41">
         <v>2000</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="122">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="D22" s="41">
         <v>1100</v>
       </c>
-      <c r="E22" s="41">
-        <v>600</v>
+      <c r="E22" s="122">
+        <f t="shared" si="1"/>
+        <v>500</v>
       </c>
       <c r="F22" s="41">
         <v>600</v>
@@ -78053,7 +78238,7 @@
         <v>600</v>
       </c>
       <c r="H22" s="41">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="I22" s="41">
         <v>500</v>
@@ -78076,81 +78261,89 @@
       <c r="O22" s="41">
         <v>500</v>
       </c>
-      <c r="P22" s="41">
+      <c r="P22" s="122">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="Q22" s="41">
+        <v>500</v>
+      </c>
+      <c r="R22" s="41">
         <v>400</v>
       </c>
-      <c r="Q22" s="41">
+      <c r="S22" s="41">
         <v>400</v>
-      </c>
-      <c r="R22" s="41">
-        <v>300</v>
-      </c>
-      <c r="S22" s="41">
-        <v>300</v>
       </c>
       <c r="T22" s="41">
         <v>300</v>
       </c>
       <c r="U22" s="41">
+        <v>300</v>
+      </c>
+      <c r="V22" s="41">
+        <v>300</v>
+      </c>
+      <c r="W22" s="41">
         <v>200</v>
       </c>
-      <c r="V22" s="41">
+      <c r="X22" s="41">
         <v>100</v>
       </c>
-      <c r="W22" s="41">
+      <c r="Y22" s="41">
         <v>100</v>
       </c>
-      <c r="X22" s="41">
+      <c r="Z22" s="41">
         <v>0</v>
       </c>
-      <c r="Y22" s="42">
+      <c r="AA22" s="42">
         <v>2000</v>
       </c>
-      <c r="Z22" s="45">
-        <f t="shared" si="1"/>
+      <c r="AB22" s="45">
+        <f t="shared" si="3"/>
         <v>2300</v>
-      </c>
-      <c r="AA22" s="41">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="AB22" s="41">
-        <f t="shared" si="3"/>
-        <v>0.3</v>
       </c>
       <c r="AC22" s="41">
         <f t="shared" si="4"/>
-        <v>0.55000000000000004</v>
+        <v>0.25</v>
       </c>
       <c r="AD22" s="41">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="AE22" s="41">
         <f t="shared" si="6"/>
-        <v>3.3333333333333335</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AF22" s="41">
         <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="AG22" s="41">
+        <f t="shared" si="8"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="AH22" s="41">
+        <f>6000/D22</f>
         <v>5.4545454545454541</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:34">
       <c r="A23">
         <v>201512</v>
       </c>
       <c r="B23">
         <v>1900</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="122">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="D23">
         <v>1000</v>
       </c>
-      <c r="E23">
-        <v>700</v>
+      <c r="E23" s="122">
+        <f t="shared" si="1"/>
+        <v>300</v>
       </c>
       <c r="F23">
         <v>700</v>
@@ -78159,7 +78352,7 @@
         <v>700</v>
       </c>
       <c r="H23">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="I23">
         <v>600</v>
@@ -78168,7 +78361,7 @@
         <v>600</v>
       </c>
       <c r="K23">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="L23">
         <v>500</v>
@@ -78177,13 +78370,14 @@
         <v>500</v>
       </c>
       <c r="N23">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="O23">
         <v>400</v>
       </c>
-      <c r="P23">
-        <v>400</v>
+      <c r="P23" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
       </c>
       <c r="Q23">
         <v>400</v>
@@ -78192,71 +78386,78 @@
         <v>400</v>
       </c>
       <c r="S23">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="T23">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="U23">
         <v>300</v>
       </c>
       <c r="V23">
+        <v>300</v>
+      </c>
+      <c r="W23">
+        <v>300</v>
+      </c>
+      <c r="X23">
         <v>200</v>
       </c>
-      <c r="W23">
+      <c r="Y23">
         <v>100</v>
       </c>
-      <c r="X23">
+      <c r="Z23">
         <v>100</v>
       </c>
-      <c r="Y23" s="39">
+      <c r="AA23" s="39">
         <v>1900</v>
       </c>
-      <c r="Z23" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB23" s="44">
+        <f t="shared" si="3"/>
         <v>2200</v>
-      </c>
-      <c r="AA23">
-        <f t="shared" si="2"/>
-        <v>0.21052631578947367</v>
-      </c>
-      <c r="AB23">
-        <f t="shared" si="3"/>
-        <v>0.36842105263157893</v>
       </c>
       <c r="AC23">
         <f t="shared" si="4"/>
-        <v>0.52631578947368418</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="AD23">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>0.36842105263157893</v>
       </c>
       <c r="AE23">
         <f t="shared" si="6"/>
-        <v>2.8571428571428572</v>
+        <v>0.52631578947368418</v>
       </c>
       <c r="AF23">
         <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="AG23">
+        <f t="shared" si="8"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="AH23">
+        <f>6000/D23</f>
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:34">
       <c r="A24">
         <v>201601</v>
       </c>
       <c r="B24">
         <v>1600</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="122">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="D24">
         <v>700</v>
       </c>
-      <c r="E24">
-        <v>400</v>
+      <c r="E24" s="122">
+        <f t="shared" si="1"/>
+        <v>300</v>
       </c>
       <c r="F24">
         <v>400</v>
@@ -78268,7 +78469,7 @@
         <v>400</v>
       </c>
       <c r="I24">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="J24">
         <v>300</v>
@@ -78277,7 +78478,7 @@
         <v>300</v>
       </c>
       <c r="L24">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="M24">
         <v>200</v>
@@ -78286,10 +78487,11 @@
         <v>200</v>
       </c>
       <c r="O24">
-        <v>100</v>
-      </c>
-      <c r="P24">
-        <v>100</v>
+        <v>200</v>
+      </c>
+      <c r="P24" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
       </c>
       <c r="Q24">
         <v>100</v>
@@ -78298,10 +78500,10 @@
         <v>100</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -78315,303 +78517,730 @@
       <c r="X24">
         <v>0</v>
       </c>
-      <c r="Y24" s="39">
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="39">
         <v>1600</v>
       </c>
-      <c r="Z24" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB24" s="44">
+        <f t="shared" si="3"/>
         <v>1900</v>
-      </c>
-      <c r="AA24">
-        <f t="shared" si="2"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="AB24">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
       </c>
       <c r="AC24">
         <f t="shared" si="4"/>
-        <v>0.4375</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AD24">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>0.25</v>
       </c>
       <c r="AE24">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0.4375</v>
       </c>
       <c r="AF24">
         <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AG24">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AH24">
+        <f>6000/D24</f>
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:34">
       <c r="A25">
         <v>201602</v>
       </c>
       <c r="B25">
         <v>2600</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="122">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="D25">
         <v>1700</v>
       </c>
-      <c r="E25">
-        <v>1000</v>
+      <c r="E25" s="122">
+        <f t="shared" si="1"/>
+        <v>700</v>
       </c>
       <c r="F25">
         <v>1000</v>
       </c>
       <c r="G25">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="H25">
         <v>900</v>
       </c>
       <c r="I25">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="J25">
         <v>800</v>
       </c>
       <c r="K25">
+        <v>800</v>
+      </c>
+      <c r="L25">
         <v>700</v>
-      </c>
-      <c r="L25">
-        <v>600</v>
       </c>
       <c r="M25">
         <v>600</v>
       </c>
       <c r="N25">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="O25">
         <v>500</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="122">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="Q25">
+        <v>500</v>
+      </c>
+      <c r="R25">
         <v>400</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <v>300</v>
-      </c>
-      <c r="R25">
-        <v>200</v>
-      </c>
-      <c r="S25">
-        <v>200</v>
       </c>
       <c r="T25">
         <v>200</v>
       </c>
       <c r="U25">
+        <v>200</v>
+      </c>
+      <c r="V25">
+        <v>200</v>
+      </c>
+      <c r="W25">
         <v>100</v>
       </c>
-      <c r="V25">
+      <c r="X25">
         <v>100</v>
       </c>
-      <c r="W25">
+      <c r="Y25">
         <v>0</v>
       </c>
-      <c r="X25">
+      <c r="Z25">
         <v>0</v>
       </c>
-      <c r="Y25" s="39">
+      <c r="AA25" s="39">
         <v>2600</v>
       </c>
-      <c r="Z25" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB25" s="44">
+        <f t="shared" si="3"/>
         <v>2900</v>
-      </c>
-      <c r="AA25">
-        <f t="shared" si="2"/>
-        <v>0.19230769230769232</v>
-      </c>
-      <c r="AB25">
-        <f t="shared" si="3"/>
-        <v>0.38461538461538464</v>
       </c>
       <c r="AC25">
         <f t="shared" si="4"/>
-        <v>0.65384615384615385</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="AD25">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="AE25">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0.65384615384615385</v>
       </c>
       <c r="AF25">
         <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="AH25">
+        <f>6000/D25</f>
         <v>3.5294117647058822</v>
       </c>
     </row>
-    <row r="26" spans="1:32">
-      <c r="A26">
+    <row r="26" spans="1:34" s="55" customFormat="1">
+      <c r="A26" s="55">
         <v>201603</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="55">
         <v>2500</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="122">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="55">
         <v>1600</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="122">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="F26" s="55">
         <v>1000</v>
       </c>
-      <c r="F26">
+      <c r="G26" s="55">
         <v>1000</v>
       </c>
-      <c r="G26">
+      <c r="H26" s="55">
+        <v>1000</v>
+      </c>
+      <c r="I26" s="55">
+        <v>1000</v>
+      </c>
+      <c r="J26" s="55">
         <v>900</v>
       </c>
-      <c r="H26">
+      <c r="K26" s="55">
         <v>900</v>
       </c>
-      <c r="I26">
+      <c r="L26" s="55">
         <v>900</v>
       </c>
-      <c r="J26">
+      <c r="M26" s="55">
         <v>800</v>
       </c>
-      <c r="K26">
+      <c r="N26" s="55">
         <v>800</v>
       </c>
-      <c r="L26">
+      <c r="O26" s="55">
         <v>700</v>
       </c>
-      <c r="M26">
+      <c r="P26" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="Q26" s="55">
+        <v>700</v>
+      </c>
+      <c r="R26" s="55">
         <v>600</v>
       </c>
-      <c r="N26">
+      <c r="S26" s="55">
         <v>500</v>
       </c>
-      <c r="O26">
-        <v>500</v>
-      </c>
-      <c r="P26">
-        <v>500</v>
-      </c>
-      <c r="Q26">
+      <c r="T26" s="55">
+        <v>400</v>
+      </c>
+      <c r="U26" s="55">
         <v>300</v>
       </c>
-      <c r="R26">
-        <v>300</v>
-      </c>
-      <c r="S26">
+      <c r="V26" s="55">
         <v>200</v>
       </c>
-      <c r="T26">
+      <c r="W26" s="55">
+        <v>200</v>
+      </c>
+      <c r="X26" s="55">
+        <v>200</v>
+      </c>
+      <c r="Y26" s="55">
         <v>100</v>
       </c>
-      <c r="U26">
-        <v>100</v>
-      </c>
-      <c r="V26">
-        <v>100</v>
-      </c>
-      <c r="W26">
+      <c r="Z26" s="55">
         <v>0</v>
       </c>
-      <c r="X26">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="39">
+      <c r="AA26" s="120">
         <v>2500</v>
       </c>
-      <c r="Z26" s="44">
-        <f t="shared" si="1"/>
+      <c r="AB26" s="121">
+        <f t="shared" si="3"/>
         <v>2800</v>
       </c>
-      <c r="AA26">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="AB26">
-        <f t="shared" si="3"/>
+      <c r="AC26" s="55">
+        <f t="shared" si="4"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AD26" s="55">
+        <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
-      <c r="AC26">
-        <f t="shared" si="4"/>
+      <c r="AE26" s="55">
+        <f t="shared" si="6"/>
         <v>0.64</v>
       </c>
-      <c r="AD26">
-        <f t="shared" si="5"/>
+      <c r="AF26" s="55">
+        <f t="shared" si="7"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="AG26" s="55">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="AE26">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="AF26">
-        <f t="shared" si="7"/>
+      <c r="AH26" s="55">
+        <f>6000/D26</f>
         <v>3.75</v>
       </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:34">
       <c r="A27">
         <v>201604</v>
       </c>
       <c r="B27">
         <v>2300</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="122">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="D27">
         <v>1400</v>
       </c>
-      <c r="AF27">
+      <c r="E27" s="122">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="F27">
+        <v>1100</v>
+      </c>
+      <c r="G27">
+        <v>1000</v>
+      </c>
+      <c r="H27">
+        <v>1000</v>
+      </c>
+      <c r="I27">
+        <v>900</v>
+      </c>
+      <c r="J27">
+        <v>900</v>
+      </c>
+      <c r="K27">
+        <v>900</v>
+      </c>
+      <c r="L27">
+        <v>800</v>
+      </c>
+      <c r="M27">
+        <v>800</v>
+      </c>
+      <c r="N27">
+        <v>700</v>
+      </c>
+      <c r="O27">
+        <v>700</v>
+      </c>
+      <c r="P27" s="122">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="Q27">
+        <v>700</v>
+      </c>
+      <c r="R27">
+        <v>700</v>
+      </c>
+      <c r="S27">
+        <v>600</v>
+      </c>
+      <c r="T27">
+        <v>600</v>
+      </c>
+      <c r="U27">
+        <v>600</v>
+      </c>
+      <c r="V27">
+        <v>500</v>
+      </c>
+      <c r="W27">
+        <v>500</v>
+      </c>
+      <c r="X27">
+        <v>400</v>
+      </c>
+      <c r="Y27">
+        <v>300</v>
+      </c>
+      <c r="Z27">
+        <v>100</v>
+      </c>
+      <c r="AA27">
+        <f>B27</f>
+        <v>2300</v>
+      </c>
+      <c r="AB27" s="121">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="AC27" s="55">
+        <f t="shared" si="4"/>
+        <v>0.30434782608695654</v>
+      </c>
+      <c r="AD27" s="55">
+        <f t="shared" si="5"/>
+        <v>0.47826086956521741</v>
+      </c>
+      <c r="AE27" s="55">
+        <f t="shared" si="6"/>
+        <v>0.60869565217391308</v>
+      </c>
+      <c r="AF27" s="55">
         <f t="shared" si="7"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="AG27" s="55">
+        <f t="shared" si="8"/>
+        <v>1.8181818181818181</v>
+      </c>
+      <c r="AH27" s="55">
+        <f>6000/D27</f>
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:34">
       <c r="A28">
         <v>201605</v>
       </c>
       <c r="B28">
         <v>2200</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="122">
         <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="D28">
+        <v>1400</v>
+      </c>
+      <c r="E28" s="122">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="F28">
+        <v>1000</v>
+      </c>
+      <c r="G28">
+        <v>1000</v>
+      </c>
+      <c r="H28">
+        <v>1000</v>
+      </c>
+      <c r="I28">
+        <v>1000</v>
+      </c>
+      <c r="J28">
+        <v>1000</v>
+      </c>
+      <c r="K28">
+        <v>900</v>
+      </c>
+      <c r="L28">
+        <v>900</v>
+      </c>
+      <c r="M28">
+        <v>800</v>
+      </c>
+      <c r="N28">
+        <v>700</v>
+      </c>
+      <c r="O28">
+        <v>700</v>
+      </c>
+      <c r="P28" s="122">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="Q28">
+        <v>700</v>
+      </c>
+      <c r="R28">
+        <v>600</v>
+      </c>
+      <c r="S28">
+        <v>600</v>
+      </c>
+      <c r="T28">
+        <v>600</v>
+      </c>
+      <c r="U28">
+        <v>500</v>
+      </c>
+      <c r="V28">
+        <v>500</v>
+      </c>
+      <c r="W28">
+        <v>300</v>
+      </c>
+      <c r="X28">
+        <v>300</v>
+      </c>
+      <c r="Y28">
+        <v>200</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" ref="AA28:AA30" si="9">B28</f>
         <v>2200</v>
       </c>
-    </row>
-    <row r="29" spans="1:32">
+      <c r="AB28" s="121">
+        <f t="shared" si="3"/>
+        <v>2500</v>
+      </c>
+      <c r="AC28" s="55">
+        <f t="shared" si="4"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="AD28" s="55">
+        <f t="shared" si="5"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="AE28" s="55">
+        <f t="shared" si="6"/>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="AF28" s="55">
+        <f t="shared" si="7"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="AG28" s="55">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="AH28" s="55">
+        <f>6000/D28</f>
+        <v>4.2857142857142856</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34">
       <c r="A29">
         <v>201606</v>
       </c>
       <c r="B29">
         <v>1600</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="122">
         <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="D29">
+        <v>900</v>
+      </c>
+      <c r="E29" s="122">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="F29">
+        <v>400</v>
+      </c>
+      <c r="G29">
+        <v>400</v>
+      </c>
+      <c r="H29">
+        <v>400</v>
+      </c>
+      <c r="I29">
+        <v>400</v>
+      </c>
+      <c r="J29">
+        <v>400</v>
+      </c>
+      <c r="K29">
+        <v>300</v>
+      </c>
+      <c r="L29">
+        <v>300</v>
+      </c>
+      <c r="M29">
+        <v>300</v>
+      </c>
+      <c r="N29">
+        <v>300</v>
+      </c>
+      <c r="O29">
+        <v>300</v>
+      </c>
+      <c r="P29" s="122">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="Q29">
+        <v>300</v>
+      </c>
+      <c r="R29">
+        <v>300</v>
+      </c>
+      <c r="S29">
+        <v>300</v>
+      </c>
+      <c r="T29">
+        <v>300</v>
+      </c>
+      <c r="U29">
+        <v>200</v>
+      </c>
+      <c r="V29">
+        <v>200</v>
+      </c>
+      <c r="W29">
+        <v>200</v>
+      </c>
+      <c r="X29">
+        <v>100</v>
+      </c>
+      <c r="Y29">
+        <v>100</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="9"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="30" spans="1:32">
+      <c r="AB29" s="121">
+        <f t="shared" si="3"/>
+        <v>1900</v>
+      </c>
+      <c r="AC29" s="55">
+        <f t="shared" si="4"/>
+        <v>0.1875</v>
+      </c>
+      <c r="AD29" s="55">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="AE29" s="55">
+        <f t="shared" si="6"/>
+        <v>0.5625</v>
+      </c>
+      <c r="AF29" s="55">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="AG29" s="55">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AH29" s="55">
+        <f>6000/D29</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34">
       <c r="A30">
         <v>201607</v>
       </c>
       <c r="B30">
         <v>2400</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="122">
         <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="D30">
+        <v>1800</v>
+      </c>
+      <c r="E30" s="122">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="F30">
+        <v>1100</v>
+      </c>
+      <c r="G30">
+        <v>1100</v>
+      </c>
+      <c r="H30">
+        <v>1100</v>
+      </c>
+      <c r="I30">
+        <v>1000</v>
+      </c>
+      <c r="J30">
+        <v>900</v>
+      </c>
+      <c r="K30">
+        <v>900</v>
+      </c>
+      <c r="L30">
+        <v>900</v>
+      </c>
+      <c r="M30">
+        <v>800</v>
+      </c>
+      <c r="N30">
+        <v>700</v>
+      </c>
+      <c r="O30">
+        <v>700</v>
+      </c>
+      <c r="P30" s="122">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="Q30">
+        <v>600</v>
+      </c>
+      <c r="R30">
+        <v>600</v>
+      </c>
+      <c r="S30">
+        <v>600</v>
+      </c>
+      <c r="T30">
+        <v>500</v>
+      </c>
+      <c r="U30">
+        <v>300</v>
+      </c>
+      <c r="V30">
+        <v>300</v>
+      </c>
+      <c r="W30">
+        <v>300</v>
+      </c>
+      <c r="X30">
+        <v>200</v>
+      </c>
+      <c r="Y30">
+        <v>100</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="9"/>
         <v>2400</v>
+      </c>
+      <c r="AB30" s="121">
+        <f t="shared" si="3"/>
+        <v>2700</v>
+      </c>
+      <c r="AC30" s="55">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="AD30" s="55">
+        <f t="shared" si="5"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="AE30" s="55">
+        <f t="shared" si="6"/>
+        <v>0.75</v>
+      </c>
+      <c r="AF30" s="55">
+        <f t="shared" si="7"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="AG30" s="55">
+        <f t="shared" si="8"/>
+        <v>1.8181818181818181</v>
+      </c>
+      <c r="AH30" s="55">
+        <f>6000/D30</f>
+        <v>3.3333333333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>